<commit_message>
Removed acquisition date from Sam Ramsamy collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/SAM RAMSAMY COLLECTION.xlsx
+++ b/Photographic Archive/SAM RAMSAMY COLLECTION.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>identifier</t>
   </si>
@@ -40,24 +40,9 @@
     <t>file_path</t>
   </si>
   <si>
-    <t>ACCESSION NO</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>ACQUISITION NO.</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>ITEM DESCRIPTION</t>
-  </si>
-  <si>
-    <t>LOCATION | SECTION</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -74,9 +59,6 @@
   </si>
   <si>
     <t>RAMSAMY, SAM PICTURE</t>
-  </si>
-  <si>
-    <t>01/04/2014</t>
   </si>
   <si>
     <t>PICTURE</t>
@@ -500,11 +482,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -514,8 +496,9 @@
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="8" max="9" width="92.33203125" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -545,10 +528,18 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -564,517 +555,463 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" t="s">
-        <v>55</v>
-      </c>
-      <c r="N13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" t="s">
-        <v>58</v>
-      </c>
-      <c r="N14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" t="s">
         <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>60</v>
-      </c>
-      <c r="M15" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>63</v>
-      </c>
-      <c r="M16" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>66</v>
-      </c>
-      <c r="M17" t="s">
-        <v>67</v>
-      </c>
-      <c r="N17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -1082,7 +1019,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
@@ -1090,7 +1027,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
@@ -1098,7 +1035,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
@@ -1106,7 +1043,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
@@ -1114,7 +1051,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
@@ -1122,7 +1059,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
@@ -1130,7 +1067,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
@@ -1138,7 +1075,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
@@ -1146,7 +1083,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
@@ -1154,7 +1091,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
@@ -1162,7 +1099,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
@@ -1170,7 +1107,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
@@ -1178,7 +1115,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
@@ -1186,7 +1123,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
@@ -1474,14 +1411,6 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>